<commit_message>
art subjects gendered, dod baseline established, better topic distribution
</commit_message>
<xml_diff>
--- a/main/template.xlsx
+++ b/main/template.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="dod" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">Наименование предмета: {} Преподователь: {}</t>
   </si>
@@ -90,6 +91,9 @@
   <si>
     <t xml:space="preserve">Максимальные баллы</t>
   </si>
+  <si>
+    <t xml:space="preserve">Зчт</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +105,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="dd\.mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +140,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -254,7 +265,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,7 +357,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,19 +632,21 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="2.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="5.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="1" width="6.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="45.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="20.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="20" style="2" width="12.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16369" min="34" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16370" min="16370" style="2" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16371" style="1" width="11.53"/>
@@ -644,27 +657,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
-      <c r="P1" s="0"/>
-      <c r="Q1" s="0"/>
-      <c r="R1" s="0"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="0"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
         <v>1</v>
@@ -2617,4 +2630,1490 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1:H1000"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="2.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="9" style="2" width="12.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16358" min="23" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16359" min="16359" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16360" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11"/>
+      <c r="B4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11"/>
+      <c r="B5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="n">
+        <v>17</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="n">
+        <v>19</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15" t="n">
+        <v>23</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15" t="n">
+        <v>24</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15" t="n">
+        <v>25</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="n">
+        <v>26</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="n">
+        <v>27</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="n">
+        <v>28</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="15" t="n">
+        <v>32</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15" t="n">
+        <v>33</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="n">
+        <v>34</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="n">
+        <v>35</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="n">
+        <v>36</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B5:B7"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.984027777777778" right="0.984027777777778" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
one step forward reformatted, but not resolved
</commit_message>
<xml_diff>
--- a/main/template.xlsx
+++ b/main/template.xlsx
@@ -105,7 +105,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="dd\.mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -133,6 +133,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -256,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,11 +276,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,67 +288,71 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,28 +368,32 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -633,7 +648,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -855,796 +870,796 @@
       <c r="R7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+      <c r="A8" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+      <c r="A9" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
+      <c r="A10" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
+      <c r="A11" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+      <c r="A12" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
+      <c r="A13" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
+      <c r="A14" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
+      <c r="A15" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="n">
+      <c r="A16" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="n">
+      <c r="A17" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
+      <c r="A18" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="n">
+      <c r="A19" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
+      <c r="A20" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
+      <c r="A21" s="20" t="n">
         <v>14</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+      <c r="A22" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="n">
+      <c r="A23" s="20" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="n">
+      <c r="A24" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="n">
+      <c r="A25" s="20" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="n">
+      <c r="A26" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="n">
+      <c r="A27" s="20" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="n">
+      <c r="A28" s="20" t="n">
         <v>21</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="n">
+      <c r="A29" s="20" t="n">
         <v>22</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="n">
+      <c r="A30" s="20" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="n">
+      <c r="A31" s="20" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="n">
+      <c r="A32" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="n">
+      <c r="A33" s="20" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="n">
+      <c r="A34" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="n">
+      <c r="A35" s="20" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="n">
+      <c r="A36" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="n">
+      <c r="A37" s="20" t="n">
         <v>30</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="n">
+      <c r="A38" s="20" t="n">
         <v>31</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="25"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="n">
+      <c r="A39" s="20" t="n">
         <v>32</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="n">
+      <c r="A40" s="20" t="n">
         <v>33</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="25"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="n">
+      <c r="A41" s="20" t="n">
         <v>34</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="n">
+      <c r="A42" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="25"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="n">
+      <c r="A43" s="20" t="n">
         <v>36</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2640,7 +2655,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2656,7 +2671,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="9" style="2" width="12.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16358" min="23" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16359" min="16359" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16360" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16360" style="32" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2747,400 +2762,400 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+      <c r="A8" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+      <c r="A9" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
+      <c r="A10" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
+      <c r="A11" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+      <c r="A12" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
+      <c r="A13" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
+      <c r="A14" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
+      <c r="A15" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="n">
+      <c r="A16" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="n">
+      <c r="A17" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
+      <c r="A18" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="n">
+      <c r="A19" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
+      <c r="A20" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
+      <c r="A21" s="20" t="n">
         <v>14</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+      <c r="A22" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="n">
+      <c r="A23" s="20" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="n">
+      <c r="A24" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="n">
+      <c r="A25" s="20" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="n">
+      <c r="A26" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="n">
+      <c r="A27" s="20" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="n">
+      <c r="A28" s="20" t="n">
         <v>21</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="n">
+      <c r="A29" s="20" t="n">
         <v>22</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="n">
+      <c r="A30" s="20" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="n">
+      <c r="A31" s="20" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="n">
+      <c r="A32" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="n">
+      <c r="A33" s="20" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="n">
+      <c r="A34" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="n">
+      <c r="A35" s="20" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="n">
+      <c r="A36" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="n">
+      <c r="A37" s="20" t="n">
         <v>30</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="n">
+      <c r="A38" s="20" t="n">
         <v>31</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="n">
+      <c r="A39" s="20" t="n">
         <v>32</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="n">
+      <c r="A40" s="20" t="n">
         <v>33</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="n">
+      <c r="A41" s="20" t="n">
         <v>34</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="n">
+      <c r="A42" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="n">
+      <c r="A43" s="20" t="n">
         <v>36</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
done with dods, topics, and new template format, fixed writer bug for dods
</commit_message>
<xml_diff>
--- a/main/template.xlsx
+++ b/main/template.xlsx
@@ -282,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -393,6 +393,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
@@ -1957,25 +1960,27 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
+    <row r="44" ht="22.5" customHeight="1">
+      <c r="A44" s="43">
+        <v>37.0</v>
+      </c>
+      <c r="B44" s="31"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="33"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="42"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
       <c r="S44" s="30"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
@@ -1985,25 +1990,27 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="30"/>
+    <row r="45" ht="22.5" customHeight="1">
+      <c r="A45" s="43">
+        <v>38.0</v>
+      </c>
+      <c r="B45" s="31"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="42"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
       <c r="S45" s="30"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
@@ -2013,25 +2020,27 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
+    <row r="46" ht="22.5" customHeight="1">
+      <c r="A46" s="43">
+        <v>39.0</v>
+      </c>
+      <c r="B46" s="31"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
       <c r="S46" s="30"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
@@ -2041,25 +2050,27 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="30"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="30"/>
+    <row r="47" ht="22.5" customHeight="1">
+      <c r="A47" s="43">
+        <v>40.0</v>
+      </c>
+      <c r="B47" s="31"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="42"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
       <c r="S47" s="30"/>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
@@ -2069,25 +2080,27 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
+    <row r="48" ht="22.5" customHeight="1">
+      <c r="A48" s="43">
+        <v>41.0</v>
+      </c>
+      <c r="B48" s="31"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="33"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
       <c r="S48" s="30"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
@@ -2097,25 +2110,27 @@
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="30"/>
-      <c r="R49" s="30"/>
+    <row r="49" ht="22.5" customHeight="1">
+      <c r="A49" s="43">
+        <v>42.0</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="42"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
       <c r="S49" s="30"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
@@ -2125,25 +2140,27 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30"/>
-      <c r="O50" s="30"/>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="30"/>
-      <c r="R50" s="30"/>
+    <row r="50" ht="22.5" customHeight="1">
+      <c r="A50" s="43">
+        <v>43.0</v>
+      </c>
+      <c r="B50" s="31"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="42"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
       <c r="S50" s="30"/>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
@@ -2153,25 +2170,27 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
+    <row r="51" ht="22.5" customHeight="1">
+      <c r="A51" s="43">
+        <v>44.0</v>
+      </c>
+      <c r="B51" s="31"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="42"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
       <c r="S51" s="30"/>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
@@ -2181,25 +2200,27 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="30"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30"/>
-      <c r="O52" s="30"/>
-      <c r="P52" s="30"/>
-      <c r="Q52" s="30"/>
-      <c r="R52" s="30"/>
+    <row r="52" ht="22.5" customHeight="1">
+      <c r="A52" s="43">
+        <v>45.0</v>
+      </c>
+      <c r="B52" s="31"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="42"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
       <c r="S52" s="30"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
@@ -2209,25 +2230,27 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
+    <row r="53" ht="22.5" customHeight="1">
+      <c r="A53" s="43">
+        <v>46.0</v>
+      </c>
+      <c r="B53" s="31"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="42"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
       <c r="S53" s="30"/>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
@@ -2237,25 +2260,27 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="30"/>
-      <c r="N54" s="30"/>
-      <c r="O54" s="30"/>
-      <c r="P54" s="30"/>
-      <c r="Q54" s="30"/>
-      <c r="R54" s="30"/>
+    <row r="54" ht="22.5" customHeight="1">
+      <c r="A54" s="43">
+        <v>47.0</v>
+      </c>
+      <c r="B54" s="31"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="42"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
       <c r="S54" s="30"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
@@ -2265,25 +2290,27 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="30"/>
+    <row r="55" ht="22.5" customHeight="1">
+      <c r="A55" s="43">
+        <v>48.0</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="33"/>
+      <c r="P55" s="42"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
       <c r="S55" s="30"/>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
@@ -2293,25 +2320,27 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
-      <c r="L56" s="30"/>
-      <c r="M56" s="30"/>
-      <c r="N56" s="30"/>
-      <c r="O56" s="30"/>
-      <c r="P56" s="30"/>
-      <c r="Q56" s="30"/>
-      <c r="R56" s="30"/>
+    <row r="56" ht="22.5" customHeight="1">
+      <c r="A56" s="43">
+        <v>49.0</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="34"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="33"/>
+      <c r="O56" s="33"/>
+      <c r="P56" s="42"/>
+      <c r="Q56" s="37"/>
+      <c r="R56" s="37"/>
       <c r="S56" s="30"/>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
@@ -2321,25 +2350,27 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
-      <c r="M57" s="30"/>
-      <c r="N57" s="30"/>
-      <c r="O57" s="30"/>
-      <c r="P57" s="30"/>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="30"/>
+    <row r="57" ht="22.5" customHeight="1">
+      <c r="A57" s="43">
+        <v>50.0</v>
+      </c>
+      <c r="B57" s="31"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
+      <c r="N57" s="33"/>
+      <c r="O57" s="33"/>
+      <c r="P57" s="42"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
       <c r="S57" s="30"/>
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
@@ -2349,25 +2380,27 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="30"/>
-      <c r="J58" s="30"/>
-      <c r="K58" s="30"/>
-      <c r="L58" s="30"/>
-      <c r="M58" s="30"/>
-      <c r="N58" s="30"/>
-      <c r="O58" s="30"/>
-      <c r="P58" s="30"/>
-      <c r="Q58" s="30"/>
-      <c r="R58" s="30"/>
+    <row r="58" ht="22.5" customHeight="1">
+      <c r="A58" s="43">
+        <v>51.0</v>
+      </c>
+      <c r="B58" s="31"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+      <c r="N58" s="33"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="42"/>
+      <c r="Q58" s="37"/>
+      <c r="R58" s="37"/>
       <c r="S58" s="30"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
@@ -2377,25 +2410,27 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="30"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="30"/>
-      <c r="O59" s="30"/>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="30"/>
-      <c r="R59" s="30"/>
+    <row r="59" ht="22.5" customHeight="1">
+      <c r="A59" s="43">
+        <v>52.0</v>
+      </c>
+      <c r="B59" s="31"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="33"/>
+      <c r="O59" s="33"/>
+      <c r="P59" s="42"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
       <c r="S59" s="30"/>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
@@ -28724,34 +28759,6 @@
       <c r="X999" s="3"/>
       <c r="Y999" s="3"/>
       <c r="Z999" s="3"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="A1000" s="30"/>
-      <c r="B1000" s="30"/>
-      <c r="C1000" s="30"/>
-      <c r="D1000" s="30"/>
-      <c r="E1000" s="30"/>
-      <c r="F1000" s="30"/>
-      <c r="G1000" s="30"/>
-      <c r="H1000" s="30"/>
-      <c r="I1000" s="30"/>
-      <c r="J1000" s="30"/>
-      <c r="K1000" s="30"/>
-      <c r="L1000" s="30"/>
-      <c r="M1000" s="30"/>
-      <c r="N1000" s="30"/>
-      <c r="O1000" s="30"/>
-      <c r="P1000" s="30"/>
-      <c r="Q1000" s="30"/>
-      <c r="R1000" s="30"/>
-      <c r="S1000" s="30"/>
-      <c r="T1000" s="3"/>
-      <c r="U1000" s="3"/>
-      <c r="V1000" s="3"/>
-      <c r="W1000" s="3"/>
-      <c r="X1000" s="3"/>
-      <c r="Y1000" s="3"/>
-      <c r="Z1000" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -29018,8 +29025,8 @@
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
       <c r="E8" s="35"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -29048,8 +29055,8 @@
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
       <c r="E9" s="38"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -29078,8 +29085,8 @@
       <c r="C10" s="32"/>
       <c r="D10" s="33"/>
       <c r="E10" s="38"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -29108,8 +29115,8 @@
       <c r="C11" s="32"/>
       <c r="D11" s="33"/>
       <c r="E11" s="38"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -29138,8 +29145,8 @@
       <c r="C12" s="39"/>
       <c r="D12" s="33"/>
       <c r="E12" s="38"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -29168,8 +29175,8 @@
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
       <c r="E13" s="38"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -29198,8 +29205,8 @@
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
       <c r="E14" s="38"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -29228,8 +29235,8 @@
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
       <c r="E15" s="38"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -29258,8 +29265,8 @@
       <c r="C16" s="40"/>
       <c r="D16" s="33"/>
       <c r="E16" s="38"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -29288,8 +29295,8 @@
       <c r="C17" s="41"/>
       <c r="D17" s="33"/>
       <c r="E17" s="38"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -29318,8 +29325,8 @@
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
       <c r="E18" s="38"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -29348,8 +29355,8 @@
       <c r="C19" s="32"/>
       <c r="D19" s="33"/>
       <c r="E19" s="38"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -29378,8 +29385,8 @@
       <c r="C20" s="32"/>
       <c r="D20" s="33"/>
       <c r="E20" s="38"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -29408,8 +29415,8 @@
       <c r="C21" s="32"/>
       <c r="D21" s="33"/>
       <c r="E21" s="38"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -29438,8 +29445,8 @@
       <c r="C22" s="39"/>
       <c r="D22" s="33"/>
       <c r="E22" s="38"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -29468,8 +29475,8 @@
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
       <c r="E23" s="38"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -29498,8 +29505,8 @@
       <c r="C24" s="40"/>
       <c r="D24" s="33"/>
       <c r="E24" s="38"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -29528,8 +29535,8 @@
       <c r="C25" s="40"/>
       <c r="D25" s="33"/>
       <c r="E25" s="38"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -29558,8 +29565,8 @@
       <c r="C26" s="32"/>
       <c r="D26" s="33"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -29588,8 +29595,8 @@
       <c r="C27" s="39"/>
       <c r="D27" s="33"/>
       <c r="E27" s="38"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -29618,8 +29625,8 @@
       <c r="C28" s="32"/>
       <c r="D28" s="33"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -29648,8 +29655,8 @@
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -29678,8 +29685,8 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -29708,8 +29715,8 @@
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -29738,8 +29745,8 @@
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -29768,8 +29775,8 @@
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -29798,8 +29805,8 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -29828,8 +29835,8 @@
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -29858,8 +29865,8 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -29888,8 +29895,8 @@
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
@@ -29918,8 +29925,8 @@
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="42"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -29948,8 +29955,8 @@
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -29978,8 +29985,8 @@
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="42"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -30008,8 +30015,8 @@
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="42"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -30038,8 +30045,8 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="42"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -30068,8 +30075,8 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="42"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>

</xml_diff>